<commit_message>
Fix Excel import functionality for admin users
</commit_message>
<xml_diff>
--- a/static/schedule_template.xlsx
+++ b/static/schedule_template.xlsx
@@ -1,43 +1,217 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Schedule Template" sheetId="1" r:id="rId1"/>
+    <sheet name="Instructions" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Assignment</t>
+  </si>
+  <si>
+    <t>Start Time</t>
+  </si>
+  <si>
+    <t>End Time</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Participants</t>
+  </si>
+  <si>
+    <t>admin1</t>
+  </si>
+  <si>
+    <t>admin2</t>
+  </si>
+  <si>
+    <t>admin3</t>
+  </si>
+  <si>
+    <t>Training Session A</t>
+  </si>
+  <si>
+    <t>Training Session B</t>
+  </si>
+  <si>
+    <t>Evaluation Session</t>
+  </si>
+  <si>
+    <t>05/21/2025 12:30 PM</t>
+  </si>
+  <si>
+    <t>05/21/2025 02:30 PM</t>
+  </si>
+  <si>
+    <t>05/22/2025 12:30 PM</t>
+  </si>
+  <si>
+    <t>05/21/2025 01:30 PM</t>
+  </si>
+  <si>
+    <t>05/21/2025 03:30 PM</t>
+  </si>
+  <si>
+    <t>05/22/2025 01:30 PM</t>
+  </si>
+  <si>
+    <t>Scheduled</t>
+  </si>
+  <si>
+    <t>Student1, Student2</t>
+  </si>
+  <si>
+    <t>Student3, Student4</t>
+  </si>
+  <si>
+    <t>Student5</t>
+  </si>
+  <si>
+    <t>TransDev Schedule Import Template</t>
+  </si>
+  <si>
+    <t>TransDev Schedule Import Instructions</t>
+  </si>
+  <si>
+    <t>Required Columns</t>
+  </si>
+  <si>
+    <t>The following columns are required for the import to work correctly:</t>
+  </si>
+  <si>
+    <t>• Employee: Username of an existing employee in the system (admin1, admin2, admin3, etc.)</t>
+  </si>
+  <si>
+    <t>• Assignment: Description of the training or work assignment</t>
+  </si>
+  <si>
+    <t>• Start Time: Start date and time in MM/DD/YYYY HH:MM AM/PM format</t>
+  </si>
+  <si>
+    <t>• End Time: End date and time in MM/DD/YYYY HH:MM AM/PM format</t>
+  </si>
+  <si>
+    <t>• Status: Current status of the shift (Scheduled, Swap Requested, Approved)</t>
+  </si>
+  <si>
+    <t>• Participants: Optional: List of participants/students involved in this shift</t>
+  </si>
+  <si>
+    <t>Import Process</t>
+  </si>
+  <si>
+    <t>1. Fill out the Schedule Template sheet with your data. You can copy data from another source or enter it directly.</t>
+  </si>
+  <si>
+    <t>2. Make sure all required fields are filled in and in the correct format.</t>
+  </si>
+  <si>
+    <t>3. Save this Excel file to your computer.</t>
+  </si>
+  <si>
+    <t>4. Go to the TransDev Spreadsheet View page.</t>
+  </si>
+  <si>
+    <t>5. Click the "Import Excel" button and select this file.</t>
+  </si>
+  <si>
+    <t>6. The system will process your data and add it to the schedule.</t>
+  </si>
+  <si>
+    <t>Notes and Troubleshooting</t>
+  </si>
+  <si>
+    <t>• Only admin users (admin1, admin2, admin3) can import data.</t>
+  </si>
+  <si>
+    <t>• Dates must be in MM/DD/YYYY HH:MM AM/PM format (e.g., 05/21/2025 10:30 AM).</t>
+  </si>
+  <si>
+    <t>• Employee names must match exactly with existing users in the system.</t>
+  </si>
+  <si>
+    <t>• If you get errors during import, check that your data matches the required format.</t>
+  </si>
+  <si>
+    <t>• The ID column is optional. If provided, the system will update existing shifts instead of creating new ones.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy hh:mm AM/PM"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="5">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF1F497D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF1F497D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8E4BC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -49,94 +223,44 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -424,78 +548,241 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="4" width="20.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>employee_id</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>assignment</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>start_time</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>end_time</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>students</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="1" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Sample Training</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>45797.79037644687</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>45797.87370978021</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Scheduled</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Student1, Student2</t>
-        </is>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2">
+      <c r="B1" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2">
+      <c r="B9" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2">
+      <c r="B10" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
+      <c r="B15" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2">
+      <c r="B16" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>